<commit_message>
verifysim run on the final version of the diplexer
</commit_message>
<xml_diff>
--- a/masks/code/corwin_spreadsheet_20180829.xlsx
+++ b/masks/code/corwin_spreadsheet_20180829.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patches" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="110">
   <si>
     <t xml:space="preserve">AGA Marks</t>
   </si>
@@ -476,10 +476,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:AA65536"/>
+  <dimension ref="A4:AB65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,9 +498,9 @@
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="21" min="20" style="0" width="6"/>
     <col collapsed="false" hidden="false" max="25" min="23" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="27" min="26" style="0" width="6"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,6 +535,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
@@ -578,6 +579,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -621,6 +623,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
@@ -658,6 +661,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
@@ -687,6 +691,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
@@ -716,6 +721,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
@@ -745,6 +751,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
@@ -774,6 +781,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
@@ -807,6 +815,7 @@
         <v>8</v>
       </c>
       <c r="AA12" s="2"/>
+      <c r="AB12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
@@ -854,6 +863,7 @@
         <v>17</v>
       </c>
       <c r="AA13" s="2"/>
+      <c r="AB13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -935,6 +945,7 @@
       <c r="AA14" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AB14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -1008,6 +1019,7 @@
       </c>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -1079,6 +1091,7 @@
       </c>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -1150,6 +1163,7 @@
       </c>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -1221,6 +1235,7 @@
       </c>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -1292,6 +1307,7 @@
       </c>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -1363,6 +1379,7 @@
       </c>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -1434,6 +1451,7 @@
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -1505,6 +1523,7 @@
       </c>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -1576,6 +1595,7 @@
       </c>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -1647,6 +1667,7 @@
       </c>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -1718,6 +1739,7 @@
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -1789,6 +1811,7 @@
       </c>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -1860,6 +1883,7 @@
       </c>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -1931,6 +1955,7 @@
       </c>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -2000,10 +2025,11 @@
       <c r="Y29" s="1" t="n">
         <v>23.6</v>
       </c>
-      <c r="Z29" s="1" t="s">
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -2073,10 +2099,11 @@
       <c r="Y30" s="1" t="n">
         <v>23.6</v>
       </c>
-      <c r="Z30" s="1" t="s">
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -2148,6 +2175,7 @@
       </c>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -2219,6 +2247,7 @@
       </c>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -2290,6 +2319,7 @@
       </c>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -2361,6 +2391,7 @@
       </c>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -2432,6 +2463,7 @@
       </c>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -2503,6 +2535,7 @@
       </c>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -2574,6 +2607,7 @@
       </c>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
@@ -2645,6 +2679,7 @@
       </c>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -2716,6 +2751,7 @@
       </c>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
@@ -2751,16 +2787,16 @@
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1" t="n">
-        <v>0</v>
+        <v>-12.008</v>
       </c>
       <c r="N40" s="1" t="n">
-        <v>0</v>
+        <v>5.913</v>
       </c>
       <c r="O40" s="1" t="n">
-        <v>-6.4</v>
+        <v>5.608</v>
       </c>
       <c r="P40" s="1" t="n">
-        <v>-2.724</v>
+        <v>-8.637</v>
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
@@ -2780,15 +2816,14 @@
         <v>0</v>
       </c>
       <c r="X40" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y40" s="1" t="n">
         <v>24.31</v>
       </c>
-      <c r="Z40" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
@@ -2824,16 +2859,16 @@
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1" t="n">
-        <v>0</v>
+        <v>12.008</v>
       </c>
       <c r="N41" s="1" t="n">
-        <v>0</v>
+        <v>-5.888</v>
       </c>
       <c r="O41" s="1" t="n">
-        <v>-5.8</v>
+        <v>-17.808</v>
       </c>
       <c r="P41" s="1" t="n">
-        <v>-2.449</v>
+        <v>3.439</v>
       </c>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2853,15 +2888,14 @@
         <v>0</v>
       </c>
       <c r="X41" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y41" s="1" t="n">
         <v>24.31</v>
       </c>
-      <c r="Z41" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -2897,16 +2931,16 @@
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1" t="n">
-        <v>0</v>
+        <v>12.008</v>
       </c>
       <c r="N42" s="1" t="n">
-        <v>0</v>
+        <v>6.373</v>
       </c>
       <c r="O42" s="1" t="n">
-        <v>-7</v>
+        <v>-19.008</v>
       </c>
       <c r="P42" s="1" t="n">
-        <v>-2.974</v>
+        <v>-9.347</v>
       </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -2926,15 +2960,14 @@
         <v>0</v>
       </c>
       <c r="X42" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y42" s="1" t="n">
         <v>24.31</v>
       </c>
-      <c r="Z42" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -2970,16 +3003,16 @@
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1" t="n">
-        <v>0</v>
+        <v>-12.008</v>
       </c>
       <c r="N43" s="1" t="n">
-        <v>0</v>
+        <v>18.069</v>
       </c>
       <c r="O43" s="1" t="n">
-        <v>-7</v>
+        <v>5.008</v>
       </c>
       <c r="P43" s="1" t="n">
-        <v>-2.974</v>
+        <v>-21.043</v>
       </c>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -2999,15 +3032,14 @@
         <v>0</v>
       </c>
       <c r="X43" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y43" s="1" t="n">
         <v>24.31</v>
       </c>
-      <c r="Z43" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -3079,6 +3111,7 @@
       </c>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
@@ -3150,6 +3183,7 @@
       </c>
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
+      <c r="AB45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -3221,6 +3255,7 @@
       </c>
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
+      <c r="AB46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -3292,6 +3327,7 @@
       </c>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -3363,6 +3399,7 @@
       </c>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -3434,6 +3471,7 @@
       </c>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
+      <c r="AB49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
@@ -3505,6 +3543,7 @@
       </c>
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -3576,6 +3615,7 @@
       </c>
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -3611,13 +3651,13 @@
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1" t="n">
-        <v>0</v>
+        <v>-6.901</v>
       </c>
       <c r="N52" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O52" s="1" t="n">
-        <v>-3.31</v>
+        <v>3.591</v>
       </c>
       <c r="P52" s="1" t="n">
         <v>5.139</v>
@@ -3640,15 +3680,16 @@
         <v>0</v>
       </c>
       <c r="X52" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y52" s="1" t="n">
         <v>23.6</v>
       </c>
-      <c r="Z52" s="1" t="s">
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -3720,6 +3761,7 @@
       </c>
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -3791,6 +3833,7 @@
       </c>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -3862,6 +3905,7 @@
       </c>
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
+      <c r="AB55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
@@ -3933,6 +3977,7 @@
       </c>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
@@ -4004,6 +4049,7 @@
       </c>
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
+      <c r="AB57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -4075,6 +4121,7 @@
       </c>
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -4146,6 +4193,7 @@
       </c>
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
+      <c r="AB59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -4217,6 +4265,7 @@
       </c>
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -4288,6 +4337,7 @@
       </c>
       <c r="Z61" s="1"/>
       <c r="AA61" s="1"/>
+      <c r="AB61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
@@ -4359,6 +4409,7 @@
       </c>
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
+      <c r="AB62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
@@ -4397,13 +4448,13 @@
         <v>0</v>
       </c>
       <c r="N63" s="1" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="O63" s="1" t="n">
         <v>1</v>
       </c>
       <c r="P63" s="1" t="n">
-        <v>-2.2</v>
+        <v>-2.199</v>
       </c>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
@@ -4428,10 +4479,11 @@
       <c r="Y63" s="1" t="n">
         <v>11.16</v>
       </c>
-      <c r="Z63" s="1" t="s">
+      <c r="Z63" s="1"/>
+      <c r="AA63" s="1"/>
+      <c r="AB63" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
@@ -4503,6 +4555,7 @@
       </c>
       <c r="Z64" s="1"/>
       <c r="AA64" s="1"/>
+      <c r="AB64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
@@ -4538,16 +4591,16 @@
       </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1" t="n">
-        <v>0</v>
+        <v>-5.6</v>
       </c>
       <c r="N65" s="1" t="n">
-        <v>0</v>
+        <v>-0.011</v>
       </c>
       <c r="O65" s="1" t="n">
-        <v>4</v>
+        <v>9.6</v>
       </c>
       <c r="P65" s="1" t="n">
-        <v>5</v>
+        <v>5.011</v>
       </c>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
@@ -4567,15 +4620,16 @@
         <v>0</v>
       </c>
       <c r="X65" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y65" s="1" t="n">
         <v>7.44</v>
       </c>
-      <c r="Z65" s="1" t="s">
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
@@ -4611,16 +4665,16 @@
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1" t="n">
-        <v>0</v>
+        <v>5.579</v>
       </c>
       <c r="N66" s="1" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="O66" s="1" t="n">
-        <v>4</v>
+        <v>-1.579</v>
       </c>
       <c r="P66" s="1" t="n">
-        <v>-3.55</v>
+        <v>-3.553</v>
       </c>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
@@ -4640,15 +4694,16 @@
         <v>0</v>
       </c>
       <c r="X66" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y66" s="1" t="n">
         <v>7.44</v>
       </c>
-      <c r="Z66" s="1" t="s">
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
@@ -4720,6 +4775,7 @@
       </c>
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
@@ -4791,6 +4847,7 @@
       </c>
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
+      <c r="AB68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -4826,13 +4883,13 @@
       </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1" t="n">
-        <v>0</v>
+        <v>6.908</v>
       </c>
       <c r="N69" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O69" s="1" t="n">
-        <v>2.674</v>
+        <v>-4.234</v>
       </c>
       <c r="P69" s="1" t="n">
         <v>4.291</v>
@@ -4855,15 +4912,16 @@
         <v>0</v>
       </c>
       <c r="X69" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="Y69" s="1" t="n">
         <v>23.6</v>
       </c>
-      <c r="Z69" s="1" t="s">
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
@@ -4935,6 +4993,7 @@
       </c>
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
@@ -5006,6 +5065,7 @@
       </c>
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
+      <c r="AB71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
@@ -5077,6 +5137,7 @@
       </c>
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
+      <c r="AB72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
@@ -5148,6 +5209,7 @@
       </c>
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
+      <c r="AB73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
@@ -5219,6 +5281,7 @@
       </c>
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
@@ -5290,6 +5353,7 @@
       </c>
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
@@ -5361,6 +5425,7 @@
       </c>
       <c r="Z76" s="1"/>
       <c r="AA76" s="1"/>
+      <c r="AB76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
@@ -5432,6 +5497,7 @@
       </c>
       <c r="Z77" s="1"/>
       <c r="AA77" s="1"/>
+      <c r="AB77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
@@ -5503,6 +5569,7 @@
       </c>
       <c r="Z78" s="1"/>
       <c r="AA78" s="1"/>
+      <c r="AB78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
@@ -5574,6 +5641,7 @@
       </c>
       <c r="Z79" s="1"/>
       <c r="AA79" s="1"/>
+      <c r="AB79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
@@ -5645,6 +5713,7 @@
       </c>
       <c r="Z80" s="1"/>
       <c r="AA80" s="1"/>
+      <c r="AB80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
@@ -5716,6 +5785,7 @@
       </c>
       <c r="Z81" s="1"/>
       <c r="AA81" s="1"/>
+      <c r="AB81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
@@ -5787,6 +5857,7 @@
       </c>
       <c r="Z82" s="1"/>
       <c r="AA82" s="1"/>
+      <c r="AB82" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
@@ -5858,6 +5929,7 @@
       </c>
       <c r="Z83" s="1"/>
       <c r="AA83" s="1"/>
+      <c r="AB83" s="1"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
@@ -5929,6 +6001,7 @@
       </c>
       <c r="Z84" s="1"/>
       <c r="AA84" s="1"/>
+      <c r="AB84" s="1"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
@@ -6000,6 +6073,7 @@
       </c>
       <c r="Z85" s="1"/>
       <c r="AA85" s="1"/>
+      <c r="AB85" s="1"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
@@ -6071,6 +6145,7 @@
       </c>
       <c r="Z86" s="1"/>
       <c r="AA86" s="1"/>
+      <c r="AB86" s="1"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
@@ -6142,6 +6217,7 @@
       </c>
       <c r="Z87" s="1"/>
       <c r="AA87" s="1"/>
+      <c r="AB87" s="1"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
@@ -6213,6 +6289,7 @@
       </c>
       <c r="Z88" s="1"/>
       <c r="AA88" s="1"/>
+      <c r="AB88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
@@ -6284,6 +6361,7 @@
       </c>
       <c r="Z89" s="1"/>
       <c r="AA89" s="1"/>
+      <c r="AB89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
@@ -6355,6 +6433,7 @@
       </c>
       <c r="Z90" s="1"/>
       <c r="AA90" s="1"/>
+      <c r="AB90" s="1"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
@@ -6426,6 +6505,7 @@
       </c>
       <c r="Z91" s="1"/>
       <c r="AA91" s="1"/>
+      <c r="AB91" s="1"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
@@ -6497,6 +6577,7 @@
       </c>
       <c r="Z92" s="1"/>
       <c r="AA92" s="1"/>
+      <c r="AB92" s="1"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
@@ -6568,6 +6649,7 @@
       </c>
       <c r="Z93" s="1"/>
       <c r="AA93" s="1"/>
+      <c r="AB93" s="1"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
@@ -6639,6 +6721,7 @@
       </c>
       <c r="Z94" s="1"/>
       <c r="AA94" s="1"/>
+      <c r="AB94" s="1"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
@@ -6710,6 +6793,7 @@
       </c>
       <c r="Z95" s="1"/>
       <c r="AA95" s="1"/>
+      <c r="AB95" s="1"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
@@ -6781,6 +6865,7 @@
       </c>
       <c r="Z96" s="1"/>
       <c r="AA96" s="1"/>
+      <c r="AB96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
@@ -6852,6 +6937,7 @@
       </c>
       <c r="Z97" s="1"/>
       <c r="AA97" s="1"/>
+      <c r="AB97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
@@ -6923,6 +7009,7 @@
       </c>
       <c r="Z98" s="1"/>
       <c r="AA98" s="1"/>
+      <c r="AB98" s="1"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1"/>
@@ -6952,6 +7039,7 @@
       <c r="Y99" s="1"/>
       <c r="Z99" s="1"/>
       <c r="AA99" s="1"/>
+      <c r="AB99" s="1"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -6983,9 +7071,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA102"/>
+  <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -7005,7 +7093,7 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="27" min="19" style="0" width="6"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>
   </cols>
@@ -7168,10 +7256,10 @@
         <v>82.6</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>48.265</v>
+        <v>116.935</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-34.335</v>
+        <v>34.335</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -7213,10 +7301,10 @@
         <v>59</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>24.665</v>
+        <v>93.335</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-34.335</v>
+        <v>34.335</v>
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -7258,10 +7346,10 @@
         <v>35.4</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>23.955</v>
+        <v>46.845</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-11.445</v>
+        <v>11.445</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -7303,10 +7391,10 @@
         <v>11.8</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>0.354999999999999</v>
+        <v>23.245</v>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-11.445</v>
+        <v>11.445</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -7348,10 +7436,10 @@
         <v>-11.8</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>-0.354999999999999</v>
+        <v>-23.245</v>
       </c>
       <c r="R7" s="1" t="n">
-        <v>11.445</v>
+        <v>-11.445</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -7393,10 +7481,10 @@
         <v>-35.4</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>-23.955</v>
+        <v>-46.845</v>
       </c>
       <c r="R8" s="1" t="n">
-        <v>11.445</v>
+        <v>-11.445</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -7438,10 +7526,10 @@
         <v>-59</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>-24.665</v>
+        <v>-93.335</v>
       </c>
       <c r="R9" s="1" t="n">
-        <v>34.335</v>
+        <v>-34.335</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -7483,10 +7571,10 @@
         <v>-82.6</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>-48.265</v>
+        <v>-116.935</v>
       </c>
       <c r="R10" s="1" t="n">
-        <v>34.335</v>
+        <v>-34.335</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -7602,10 +7690,10 @@
         <v>82.6</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>48.265</v>
+        <v>116.935</v>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-34.335</v>
+        <v>34.335</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -7647,10 +7735,10 @@
         <v>59</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>24.665</v>
+        <v>93.335</v>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-34.335</v>
+        <v>34.335</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -7692,10 +7780,10 @@
         <v>35.4</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>23.955</v>
+        <v>46.845</v>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-11.445</v>
+        <v>11.445</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -7737,10 +7825,10 @@
         <v>11.8</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>0.354999999999999</v>
+        <v>23.245</v>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-11.445</v>
+        <v>11.445</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -7782,10 +7870,10 @@
         <v>-11.8</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>-0.354999999999999</v>
+        <v>-23.245</v>
       </c>
       <c r="R17" s="1" t="n">
-        <v>11.445</v>
+        <v>-11.445</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -7827,10 +7915,10 @@
         <v>-35.4</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>-23.955</v>
+        <v>-46.845</v>
       </c>
       <c r="R18" s="1" t="n">
-        <v>11.445</v>
+        <v>-11.445</v>
       </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -7872,10 +7960,10 @@
         <v>-59</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>-24.665</v>
+        <v>-93.335</v>
       </c>
       <c r="R19" s="1" t="n">
-        <v>34.335</v>
+        <v>-34.335</v>
       </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -7917,10 +8005,10 @@
         <v>-82.6</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>-48.265</v>
+        <v>-116.935</v>
       </c>
       <c r="R20" s="1" t="n">
-        <v>34.335</v>
+        <v>-34.335</v>
       </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -7992,7 +8080,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>42</v>
@@ -8001,7 +8089,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1" t="n">
         <v>0</v>
@@ -8010,10 +8098,10 @@
         <v>0</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>0</v>
+        <v>24.31</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>24.31</v>
+        <v>23.6</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="n">
@@ -8023,23 +8111,23 @@
         <v>0</v>
       </c>
       <c r="L23" s="1" t="n">
-        <v>-48.473</v>
+        <v>0</v>
       </c>
       <c r="M23" s="1" t="n">
-        <v>-48.473</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="P23" s="1" t="n">
-        <v>24.31</v>
+        <v>82.6</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>18.397</v>
+        <v>116.935</v>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-5.913</v>
+        <v>34.335</v>
       </c>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -8068,23 +8156,23 @@
         <v>0</v>
       </c>
       <c r="L24" s="1" t="n">
-        <v>-24.163</v>
+        <v>0</v>
       </c>
       <c r="M24" s="1" t="n">
-        <v>-24.163</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="P24" s="1" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>-5.913</v>
+        <v>93.335</v>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-5.913</v>
+        <v>34.335</v>
       </c>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -8113,23 +8201,23 @@
         <v>0</v>
       </c>
       <c r="L25" s="1" t="n">
-        <v>0.147</v>
+        <v>0</v>
       </c>
       <c r="M25" s="1" t="n">
-        <v>0.147</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>-24.31</v>
+        <v>35.4</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>-30.223</v>
+        <v>46.845</v>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-5.913</v>
+        <v>11.445</v>
       </c>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
@@ -8158,16 +8246,24 @@
         <v>0</v>
       </c>
       <c r="L26" s="1" t="n">
-        <v>24.457</v>
+        <v>0</v>
       </c>
       <c r="M26" s="1" t="n">
-        <v>24.457</v>
+        <v>0</v>
       </c>
       <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="O26" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P26" s="1" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="Q26" s="1" t="n">
+        <v>23.245</v>
+      </c>
+      <c r="R26" s="1" t="n">
+        <v>11.445</v>
+      </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -8193,10 +8289,18 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
+      <c r="O27" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P27" s="1" t="n">
+        <v>-11.8</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>-23.245</v>
+      </c>
+      <c r="R27" s="1" t="n">
+        <v>-11.445</v>
+      </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -8222,10 +8326,18 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
+      <c r="O28" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="P28" s="1" t="n">
+        <v>-35.4</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>-46.845</v>
+      </c>
+      <c r="R28" s="1" t="n">
+        <v>-11.445</v>
+      </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
@@ -8237,55 +8349,31 @@
       <c r="AA28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <v>24.31</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="1" t="n">
-        <v>-24.457</v>
-      </c>
-      <c r="M29" s="1" t="n">
-        <v>-24.457</v>
-      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P29" s="1" t="n">
-        <v>36.465</v>
+        <v>-59</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>42.353</v>
+        <v>-93.335</v>
       </c>
       <c r="R29" s="1" t="n">
-        <v>5.888</v>
+        <v>-34.335</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
@@ -8307,30 +8395,22 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="1" t="n">
-        <v>-0.147</v>
-      </c>
-      <c r="M30" s="1" t="n">
-        <v>-0.147</v>
-      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P30" s="1" t="n">
-        <v>12.155</v>
+        <v>-82.6</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>18.043</v>
+        <v>-116.935</v>
       </c>
       <c r="R30" s="1" t="n">
-        <v>5.888</v>
+        <v>-34.335</v>
       </c>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
@@ -8352,31 +8432,15 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="1" t="n">
-        <v>24.163</v>
-      </c>
-      <c r="M31" s="1" t="n">
-        <v>24.163</v>
-      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P31" s="1" t="n">
-        <v>-12.155</v>
-      </c>
-      <c r="Q31" s="1" t="n">
-        <v>-6.267</v>
-      </c>
-      <c r="R31" s="1" t="n">
-        <v>5.888</v>
-      </c>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -8397,31 +8461,15 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="1" t="n">
-        <v>48.473</v>
-      </c>
-      <c r="M32" s="1" t="n">
-        <v>48.473</v>
-      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P32" s="1" t="n">
-        <v>-36.465</v>
-      </c>
-      <c r="Q32" s="1" t="n">
-        <v>-30.577</v>
-      </c>
-      <c r="R32" s="1" t="n">
-        <v>5.888</v>
-      </c>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -8433,24 +8481,56 @@
       <c r="AA32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>11.16</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>11.16</v>
+      </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="J33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>-39.06</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v>-42.045</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>-2.985</v>
+      </c>
       <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
+      <c r="O33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" s="1" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <v>36.075</v>
+      </c>
+      <c r="R33" s="1" t="n">
+        <v>-2.985</v>
+      </c>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
@@ -8471,15 +8551,31 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="J34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>-27.9</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>-30.885</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <v>-2.985</v>
+      </c>
       <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
+      <c r="O34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="P34" s="1" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="Q34" s="1" t="n">
+        <v>24.915</v>
+      </c>
+      <c r="R34" s="1" t="n">
+        <v>-2.985</v>
+      </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
@@ -8491,55 +8587,39 @@
       <c r="AA34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <v>24.31</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>0</v>
+        <v>-16.74</v>
       </c>
       <c r="L35" s="1" t="n">
-        <v>-24.457</v>
+        <v>-17.735</v>
       </c>
       <c r="M35" s="1" t="n">
-        <v>-24.457</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P35" s="1" t="n">
-        <v>36.465</v>
+        <v>16.74</v>
       </c>
       <c r="Q35" s="1" t="n">
-        <v>30.092</v>
+        <v>15.745</v>
       </c>
       <c r="R35" s="1" t="n">
-        <v>-6.373</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
@@ -8562,29 +8642,29 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>0</v>
+        <v>-5.58</v>
       </c>
       <c r="L36" s="1" t="n">
-        <v>-0.147</v>
+        <v>-6.575</v>
       </c>
       <c r="M36" s="1" t="n">
-        <v>-0.147</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P36" s="1" t="n">
-        <v>12.155</v>
+        <v>5.58</v>
       </c>
       <c r="Q36" s="1" t="n">
-        <v>5.782</v>
+        <v>4.585</v>
       </c>
       <c r="R36" s="1" t="n">
-        <v>-6.373</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
@@ -8607,29 +8687,29 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>0</v>
+        <v>5.58</v>
       </c>
       <c r="L37" s="1" t="n">
-        <v>24.163</v>
+        <v>6.575</v>
       </c>
       <c r="M37" s="1" t="n">
-        <v>24.163</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P37" s="1" t="n">
-        <v>-12.155</v>
+        <v>-5.58</v>
       </c>
       <c r="Q37" s="1" t="n">
-        <v>-18.528</v>
+        <v>-4.585</v>
       </c>
       <c r="R37" s="1" t="n">
-        <v>-6.373</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
@@ -8652,29 +8732,29 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>0</v>
+        <v>16.74</v>
       </c>
       <c r="L38" s="1" t="n">
-        <v>48.473</v>
+        <v>17.735</v>
       </c>
       <c r="M38" s="1" t="n">
-        <v>48.473</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P38" s="1" t="n">
-        <v>-36.465</v>
+        <v>-16.74</v>
       </c>
       <c r="Q38" s="1" t="n">
-        <v>-42.838</v>
+        <v>-15.745</v>
       </c>
       <c r="R38" s="1" t="n">
-        <v>-6.373</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
@@ -8696,15 +8776,31 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
+      <c r="J39" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <v>30.885</v>
+      </c>
+      <c r="M39" s="1" t="n">
+        <v>2.985</v>
+      </c>
       <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
+      <c r="O39" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="P39" s="1" t="n">
+        <v>-27.9</v>
+      </c>
+      <c r="Q39" s="1" t="n">
+        <v>-24.915</v>
+      </c>
+      <c r="R39" s="1" t="n">
+        <v>2.985</v>
+      </c>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
@@ -8725,15 +8821,31 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
+      <c r="J40" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>39.06</v>
+      </c>
+      <c r="L40" s="1" t="n">
+        <v>42.045</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <v>2.985</v>
+      </c>
       <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
+      <c r="O40" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="P40" s="1" t="n">
+        <v>-39.06</v>
+      </c>
+      <c r="Q40" s="1" t="n">
+        <v>-36.075</v>
+      </c>
+      <c r="R40" s="1" t="n">
+        <v>2.985</v>
+      </c>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
@@ -8745,56 +8857,24 @@
       <c r="AA40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1" t="n">
-        <v>24.31</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K41" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="1" t="n">
-        <v>-48.473</v>
-      </c>
-      <c r="M41" s="1" t="n">
-        <v>-48.473</v>
-      </c>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
       <c r="N41" s="1"/>
-      <c r="O41" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P41" s="1" t="n">
-        <v>24.31</v>
-      </c>
-      <c r="Q41" s="1" t="n">
-        <v>6.241</v>
-      </c>
-      <c r="R41" s="1" t="n">
-        <v>-18.069</v>
-      </c>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
@@ -8815,31 +8895,15 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" s="1" t="n">
-        <v>-24.163</v>
-      </c>
-      <c r="M42" s="1" t="n">
-        <v>-24.163</v>
-      </c>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="O42" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="1" t="n">
-        <v>-18.069</v>
-      </c>
-      <c r="R42" s="1" t="n">
-        <v>-18.069</v>
-      </c>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
@@ -8851,39 +8915,55 @@
       <c r="AA42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>24.31</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>7.44</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K43" s="1" t="n">
         <v>0</v>
       </c>
       <c r="L43" s="1" t="n">
-        <v>0.147</v>
+        <v>0</v>
       </c>
       <c r="M43" s="1" t="n">
-        <v>0.147</v>
+        <v>0</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P43" s="1" t="n">
-        <v>-24.31</v>
+        <v>40.92</v>
       </c>
       <c r="Q43" s="1" t="n">
-        <v>-42.379</v>
+        <v>37.935</v>
       </c>
       <c r="R43" s="1" t="n">
-        <v>-18.069</v>
+        <v>-2.985</v>
       </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
@@ -8906,22 +8986,30 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K44" s="1" t="n">
         <v>0</v>
       </c>
       <c r="L44" s="1" t="n">
-        <v>24.457</v>
+        <v>0</v>
       </c>
       <c r="M44" s="1" t="n">
-        <v>24.457</v>
+        <v>0</v>
       </c>
       <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
+      <c r="O44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="P44" s="1" t="n">
+        <v>33.48</v>
+      </c>
+      <c r="Q44" s="1" t="n">
+        <v>30.495</v>
+      </c>
+      <c r="R44" s="1" t="n">
+        <v>-2.985</v>
+      </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
@@ -8942,15 +9030,31 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
+      <c r="J45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
+      <c r="O45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P45" s="1" t="n">
+        <v>26.04</v>
+      </c>
+      <c r="Q45" s="1" t="n">
+        <v>23.055</v>
+      </c>
+      <c r="R45" s="1" t="n">
+        <v>-2.985</v>
+      </c>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
@@ -8971,15 +9075,31 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
+      <c r="J46" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
+      <c r="O46" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P46" s="1" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="Q46" s="1" t="n">
+        <v>17.605</v>
+      </c>
+      <c r="R46" s="1" t="n">
+        <v>-0.994999999999999</v>
+      </c>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
@@ -8991,55 +9111,31 @@
       <c r="AA46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D47" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H47" s="1" t="n">
-        <v>23.6</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K47" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L47" s="1" t="n">
-        <v>-43.366</v>
-      </c>
-      <c r="M47" s="1" t="n">
-        <v>-43.366</v>
-      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P47" s="1" t="n">
-        <v>82.6</v>
+        <v>11.16</v>
       </c>
       <c r="Q47" s="1" t="n">
-        <v>48.265</v>
+        <v>10.165</v>
       </c>
       <c r="R47" s="1" t="n">
-        <v>-34.335</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
@@ -9061,30 +9157,22 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K48" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L48" s="1" t="n">
-        <v>-19.056</v>
-      </c>
-      <c r="M48" s="1" t="n">
-        <v>-19.056</v>
-      </c>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P48" s="1" t="n">
-        <v>59</v>
+        <v>3.72</v>
       </c>
       <c r="Q48" s="1" t="n">
-        <v>24.665</v>
+        <v>2.725</v>
       </c>
       <c r="R48" s="1" t="n">
-        <v>-34.335</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
@@ -9106,30 +9194,22 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K49" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L49" s="1" t="n">
-        <v>5.254</v>
-      </c>
-      <c r="M49" s="1" t="n">
-        <v>5.254</v>
-      </c>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="P49" s="1" t="n">
-        <v>35.4</v>
+        <v>-3.72</v>
       </c>
       <c r="Q49" s="1" t="n">
-        <v>23.955</v>
+        <v>-2.725</v>
       </c>
       <c r="R49" s="1" t="n">
-        <v>-11.445</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
@@ -9151,30 +9231,22 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K50" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L50" s="1" t="n">
-        <v>29.564</v>
-      </c>
-      <c r="M50" s="1" t="n">
-        <v>29.564</v>
-      </c>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P50" s="1" t="n">
-        <v>11.8</v>
+        <v>-11.16</v>
       </c>
       <c r="Q50" s="1" t="n">
-        <v>0.354999999999999</v>
+        <v>-10.165</v>
       </c>
       <c r="R50" s="1" t="n">
-        <v>-11.445</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
@@ -9202,16 +9274,16 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="P51" s="1" t="n">
-        <v>-11.8</v>
+        <v>-18.6</v>
       </c>
       <c r="Q51" s="1" t="n">
-        <v>-0.354999999999999</v>
+        <v>-17.605</v>
       </c>
       <c r="R51" s="1" t="n">
-        <v>11.445</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
@@ -9239,16 +9311,16 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="P52" s="1" t="n">
-        <v>-35.4</v>
+        <v>-26.04</v>
       </c>
       <c r="Q52" s="1" t="n">
-        <v>-23.955</v>
+        <v>-23.055</v>
       </c>
       <c r="R52" s="1" t="n">
-        <v>11.445</v>
+        <v>2.985</v>
       </c>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
@@ -9276,16 +9348,16 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="P53" s="1" t="n">
-        <v>-59</v>
+        <v>-33.48</v>
       </c>
       <c r="Q53" s="1" t="n">
-        <v>-24.665</v>
+        <v>-30.495</v>
       </c>
       <c r="R53" s="1" t="n">
-        <v>34.335</v>
+        <v>2.985</v>
       </c>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
@@ -9313,16 +9385,16 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="P54" s="1" t="n">
-        <v>-82.6</v>
+        <v>-40.92</v>
       </c>
       <c r="Q54" s="1" t="n">
-        <v>-48.265</v>
+        <v>-37.935</v>
       </c>
       <c r="R54" s="1" t="n">
-        <v>34.335</v>
+        <v>2.985</v>
       </c>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
@@ -9394,16 +9466,16 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E57" s="1" t="n">
         <v>0</v>
@@ -9412,36 +9484,36 @@
         <v>0</v>
       </c>
       <c r="G57" s="1" t="n">
-        <v>11.16</v>
+        <v>24.31</v>
       </c>
       <c r="H57" s="1" t="n">
-        <v>11.16</v>
+        <v>7.44</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="1" t="n">
-        <v>-39.06</v>
+        <v>0</v>
       </c>
       <c r="L57" s="1" t="n">
-        <v>-42.045</v>
+        <v>0</v>
       </c>
       <c r="M57" s="1" t="n">
-        <v>-2.985</v>
+        <v>0</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1" t="n">
         <v>1</v>
       </c>
       <c r="P57" s="1" t="n">
-        <v>39.06</v>
+        <v>40.92</v>
       </c>
       <c r="Q57" s="1" t="n">
-        <v>42.046</v>
+        <v>37.935</v>
       </c>
       <c r="R57" s="1" t="n">
-        <v>2.986</v>
+        <v>-2.985</v>
       </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
@@ -9467,26 +9539,26 @@
         <v>2</v>
       </c>
       <c r="K58" s="1" t="n">
-        <v>-27.9</v>
+        <v>0</v>
       </c>
       <c r="L58" s="1" t="n">
-        <v>-30.885</v>
+        <v>0</v>
       </c>
       <c r="M58" s="1" t="n">
-        <v>-2.985</v>
+        <v>0</v>
       </c>
       <c r="N58" s="1"/>
       <c r="O58" s="1" t="n">
         <v>2</v>
       </c>
       <c r="P58" s="1" t="n">
-        <v>27.9</v>
+        <v>33.48</v>
       </c>
       <c r="Q58" s="1" t="n">
-        <v>30.886</v>
+        <v>30.495</v>
       </c>
       <c r="R58" s="1" t="n">
-        <v>2.986</v>
+        <v>-2.985</v>
       </c>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
@@ -9512,26 +9584,26 @@
         <v>3</v>
       </c>
       <c r="K59" s="1" t="n">
-        <v>-16.74</v>
+        <v>0</v>
       </c>
       <c r="L59" s="1" t="n">
-        <v>-17.735</v>
+        <v>0</v>
       </c>
       <c r="M59" s="1" t="n">
-        <v>-0.994999999999999</v>
+        <v>0</v>
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1" t="n">
         <v>3</v>
       </c>
       <c r="P59" s="1" t="n">
-        <v>16.74</v>
+        <v>26.04</v>
       </c>
       <c r="Q59" s="1" t="n">
-        <v>17.736</v>
+        <v>23.055</v>
       </c>
       <c r="R59" s="1" t="n">
-        <v>0.995999999999999</v>
+        <v>-2.985</v>
       </c>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
@@ -9557,26 +9629,26 @@
         <v>4</v>
       </c>
       <c r="K60" s="1" t="n">
-        <v>-5.58</v>
+        <v>0</v>
       </c>
       <c r="L60" s="1" t="n">
-        <v>-6.575</v>
+        <v>0</v>
       </c>
       <c r="M60" s="1" t="n">
-        <v>-0.994999999999999</v>
+        <v>0</v>
       </c>
       <c r="N60" s="1"/>
       <c r="O60" s="1" t="n">
         <v>4</v>
       </c>
       <c r="P60" s="1" t="n">
-        <v>5.58</v>
+        <v>18.6</v>
       </c>
       <c r="Q60" s="1" t="n">
-        <v>6.576</v>
+        <v>17.605</v>
       </c>
       <c r="R60" s="1" t="n">
-        <v>0.995999999999999</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
@@ -9598,30 +9670,22 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
-      <c r="J61" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="K61" s="1" t="n">
-        <v>5.58</v>
-      </c>
-      <c r="L61" s="1" t="n">
-        <v>6.575</v>
-      </c>
-      <c r="M61" s="1" t="n">
-        <v>0.994999999999999</v>
-      </c>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1" t="n">
         <v>5</v>
       </c>
       <c r="P61" s="1" t="n">
-        <v>-5.58</v>
+        <v>11.16</v>
       </c>
       <c r="Q61" s="1" t="n">
-        <v>-6.574</v>
+        <v>10.165</v>
       </c>
       <c r="R61" s="1" t="n">
-        <v>-0.993999999999999</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
@@ -9643,30 +9707,22 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
-      <c r="J62" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="K62" s="1" t="n">
-        <v>16.74</v>
-      </c>
-      <c r="L62" s="1" t="n">
-        <v>17.735</v>
-      </c>
-      <c r="M62" s="1" t="n">
-        <v>0.994999999999999</v>
-      </c>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1" t="n">
         <v>6</v>
       </c>
       <c r="P62" s="1" t="n">
-        <v>-16.74</v>
+        <v>3.72</v>
       </c>
       <c r="Q62" s="1" t="n">
-        <v>-17.734</v>
+        <v>2.725</v>
       </c>
       <c r="R62" s="1" t="n">
-        <v>-0.993999999999999</v>
+        <v>-0.994999999999999</v>
       </c>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
@@ -9688,30 +9744,22 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-      <c r="J63" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="K63" s="1" t="n">
-        <v>27.9</v>
-      </c>
-      <c r="L63" s="1" t="n">
-        <v>30.885</v>
-      </c>
-      <c r="M63" s="1" t="n">
-        <v>2.985</v>
-      </c>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1" t="n">
         <v>7</v>
       </c>
       <c r="P63" s="1" t="n">
-        <v>-27.9</v>
+        <v>-3.72</v>
       </c>
       <c r="Q63" s="1" t="n">
-        <v>-30.884</v>
+        <v>-2.725</v>
       </c>
       <c r="R63" s="1" t="n">
-        <v>-2.984</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
@@ -9733,30 +9781,22 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K64" s="1" t="n">
-        <v>39.06</v>
-      </c>
-      <c r="L64" s="1" t="n">
-        <v>42.045</v>
-      </c>
-      <c r="M64" s="1" t="n">
-        <v>2.985</v>
-      </c>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1" t="n">
         <v>8</v>
       </c>
       <c r="P64" s="1" t="n">
-        <v>-39.06</v>
+        <v>-11.16</v>
       </c>
       <c r="Q64" s="1" t="n">
-        <v>-42.044</v>
+        <v>-10.165</v>
       </c>
       <c r="R64" s="1" t="n">
-        <v>-2.984</v>
+        <v>0.994999999999999</v>
       </c>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
@@ -9783,10 +9823,18 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
+      <c r="O65" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="P65" s="1" t="n">
+        <v>-18.6</v>
+      </c>
+      <c r="Q65" s="1" t="n">
+        <v>-17.605</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>0.994999999999999</v>
+      </c>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
@@ -9812,10 +9860,18 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
+      <c r="O66" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="P66" s="1" t="n">
+        <v>-26.04</v>
+      </c>
+      <c r="Q66" s="1" t="n">
+        <v>-23.055</v>
+      </c>
+      <c r="R66" s="1" t="n">
+        <v>2.985</v>
+      </c>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
@@ -9827,55 +9883,31 @@
       <c r="AA66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D67" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E67" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H67" s="1" t="n">
-        <v>7.44</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
       <c r="I67" s="1"/>
-      <c r="J67" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K67" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L67" s="1" t="n">
-        <v>-42.065</v>
-      </c>
-      <c r="M67" s="1" t="n">
-        <v>-42.065</v>
-      </c>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P67" s="1" t="n">
-        <v>40.92</v>
+        <v>-33.48</v>
       </c>
       <c r="Q67" s="1" t="n">
-        <v>43.916</v>
+        <v>-30.495</v>
       </c>
       <c r="R67" s="1" t="n">
-        <v>2.996</v>
+        <v>2.985</v>
       </c>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
@@ -9897,30 +9929,22 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
-      <c r="J68" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K68" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" s="1" t="n">
-        <v>-17.755</v>
-      </c>
-      <c r="M68" s="1" t="n">
-        <v>-17.755</v>
-      </c>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="P68" s="1" t="n">
-        <v>33.48</v>
+        <v>-40.92</v>
       </c>
       <c r="Q68" s="1" t="n">
-        <v>36.476</v>
+        <v>-37.935</v>
       </c>
       <c r="R68" s="1" t="n">
-        <v>2.996</v>
+        <v>2.985</v>
       </c>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
@@ -9942,31 +9966,15 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
-      <c r="J69" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K69" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L69" s="1" t="n">
-        <v>6.555</v>
-      </c>
-      <c r="M69" s="1" t="n">
-        <v>6.555</v>
-      </c>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
       <c r="N69" s="1"/>
-      <c r="O69" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P69" s="1" t="n">
-        <v>26.04</v>
-      </c>
-      <c r="Q69" s="1" t="n">
-        <v>29.036</v>
-      </c>
-      <c r="R69" s="1" t="n">
-        <v>2.996</v>
-      </c>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
@@ -9987,31 +9995,15 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
-      <c r="J70" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K70" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L70" s="1" t="n">
-        <v>30.865</v>
-      </c>
-      <c r="M70" s="1" t="n">
-        <v>30.865</v>
-      </c>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
       <c r="N70" s="1"/>
-      <c r="O70" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P70" s="1" t="n">
-        <v>18.6</v>
-      </c>
-      <c r="Q70" s="1" t="n">
-        <v>19.606</v>
-      </c>
-      <c r="R70" s="1" t="n">
-        <v>1.006</v>
-      </c>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
@@ -10023,31 +10015,55 @@
       <c r="AA70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1" t="n">
+        <v>24.31</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <v>23.6</v>
+      </c>
       <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
+      <c r="J71" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N71" s="1"/>
       <c r="O71" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P71" s="1" t="n">
-        <v>11.16</v>
+        <v>82.6</v>
       </c>
       <c r="Q71" s="1" t="n">
-        <v>12.166</v>
+        <v>116.935</v>
       </c>
       <c r="R71" s="1" t="n">
-        <v>1.006</v>
+        <v>34.335</v>
       </c>
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
@@ -10069,22 +10085,30 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
+      <c r="J72" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N72" s="1"/>
       <c r="O72" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P72" s="1" t="n">
-        <v>3.72</v>
+        <v>59</v>
       </c>
       <c r="Q72" s="1" t="n">
-        <v>4.726</v>
+        <v>93.335</v>
       </c>
       <c r="R72" s="1" t="n">
-        <v>1.006</v>
+        <v>34.335</v>
       </c>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
@@ -10106,22 +10130,30 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
+      <c r="J73" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P73" s="1" t="n">
-        <v>-3.72</v>
+        <v>35.4</v>
       </c>
       <c r="Q73" s="1" t="n">
-        <v>-4.704</v>
+        <v>46.845</v>
       </c>
       <c r="R73" s="1" t="n">
-        <v>-0.983999999999999</v>
+        <v>11.445</v>
       </c>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
@@ -10143,22 +10175,30 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
+      <c r="J74" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="N74" s="1"/>
       <c r="O74" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P74" s="1" t="n">
-        <v>-11.16</v>
+        <v>11.8</v>
       </c>
       <c r="Q74" s="1" t="n">
-        <v>-12.144</v>
+        <v>23.245</v>
       </c>
       <c r="R74" s="1" t="n">
-        <v>-0.983999999999999</v>
+        <v>11.445</v>
       </c>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
@@ -10186,16 +10226,16 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P75" s="1" t="n">
-        <v>-18.6</v>
+        <v>-11.8</v>
       </c>
       <c r="Q75" s="1" t="n">
-        <v>-19.584</v>
+        <v>-23.245</v>
       </c>
       <c r="R75" s="1" t="n">
-        <v>-0.983999999999999</v>
+        <v>-11.445</v>
       </c>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
@@ -10223,16 +10263,16 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P76" s="1" t="n">
-        <v>-26.04</v>
+        <v>-35.4</v>
       </c>
       <c r="Q76" s="1" t="n">
-        <v>-29.014</v>
+        <v>-46.845</v>
       </c>
       <c r="R76" s="1" t="n">
-        <v>-2.974</v>
+        <v>-11.445</v>
       </c>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
@@ -10260,16 +10300,16 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="P77" s="1" t="n">
-        <v>-33.48</v>
+        <v>-59</v>
       </c>
       <c r="Q77" s="1" t="n">
-        <v>-36.454</v>
+        <v>-93.335</v>
       </c>
       <c r="R77" s="1" t="n">
-        <v>-2.974</v>
+        <v>-34.335</v>
       </c>
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
@@ -10297,16 +10337,16 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="P78" s="1" t="n">
-        <v>-40.92</v>
+        <v>-82.6</v>
       </c>
       <c r="Q78" s="1" t="n">
-        <v>-43.894</v>
+        <v>-116.935</v>
       </c>
       <c r="R78" s="1" t="n">
-        <v>-2.974</v>
+        <v>-34.335</v>
       </c>
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
@@ -10317,958 +10357,6 @@
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
       <c r="AA78" s="1"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
-      <c r="O79" s="1"/>
-      <c r="P79" s="1"/>
-      <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
-      <c r="S79" s="1"/>
-      <c r="T79" s="1"/>
-      <c r="U79" s="1"/>
-      <c r="V79" s="1"/>
-      <c r="W79" s="1"/>
-      <c r="X79" s="1"/>
-      <c r="Y79" s="1"/>
-      <c r="Z79" s="1"/>
-      <c r="AA79" s="1"/>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-      <c r="T80" s="1"/>
-      <c r="U80" s="1"/>
-      <c r="V80" s="1"/>
-      <c r="W80" s="1"/>
-      <c r="X80" s="1"/>
-      <c r="Y80" s="1"/>
-      <c r="Z80" s="1"/>
-      <c r="AA80" s="1"/>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C81" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D81" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E81" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F81" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G81" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H81" s="1" t="n">
-        <v>7.44</v>
-      </c>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K81" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L81" s="1" t="n">
-        <v>-30.886</v>
-      </c>
-      <c r="M81" s="1" t="n">
-        <v>-30.886</v>
-      </c>
-      <c r="N81" s="1"/>
-      <c r="O81" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P81" s="1" t="n">
-        <v>40.92</v>
-      </c>
-      <c r="Q81" s="1" t="n">
-        <v>43.902</v>
-      </c>
-      <c r="R81" s="1" t="n">
-        <v>2.982</v>
-      </c>
-      <c r="S81" s="1"/>
-      <c r="T81" s="1"/>
-      <c r="U81" s="1"/>
-      <c r="V81" s="1"/>
-      <c r="W81" s="1"/>
-      <c r="X81" s="1"/>
-      <c r="Y81" s="1"/>
-      <c r="Z81" s="1"/>
-      <c r="AA81" s="1"/>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K82" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L82" s="1" t="n">
-        <v>-6.576</v>
-      </c>
-      <c r="M82" s="1" t="n">
-        <v>-6.576</v>
-      </c>
-      <c r="N82" s="1"/>
-      <c r="O82" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P82" s="1" t="n">
-        <v>33.48</v>
-      </c>
-      <c r="Q82" s="1" t="n">
-        <v>36.462</v>
-      </c>
-      <c r="R82" s="1" t="n">
-        <v>2.982</v>
-      </c>
-      <c r="S82" s="1"/>
-      <c r="T82" s="1"/>
-      <c r="U82" s="1"/>
-      <c r="V82" s="1"/>
-      <c r="W82" s="1"/>
-      <c r="X82" s="1"/>
-      <c r="Y82" s="1"/>
-      <c r="Z82" s="1"/>
-      <c r="AA82" s="1"/>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K83" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L83" s="1" t="n">
-        <v>17.734</v>
-      </c>
-      <c r="M83" s="1" t="n">
-        <v>17.734</v>
-      </c>
-      <c r="N83" s="1"/>
-      <c r="O83" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P83" s="1" t="n">
-        <v>26.04</v>
-      </c>
-      <c r="Q83" s="1" t="n">
-        <v>29.022</v>
-      </c>
-      <c r="R83" s="1" t="n">
-        <v>2.982</v>
-      </c>
-      <c r="S83" s="1"/>
-      <c r="T83" s="1"/>
-      <c r="U83" s="1"/>
-      <c r="V83" s="1"/>
-      <c r="W83" s="1"/>
-      <c r="X83" s="1"/>
-      <c r="Y83" s="1"/>
-      <c r="Z83" s="1"/>
-      <c r="AA83" s="1"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K84" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L84" s="1" t="n">
-        <v>42.044</v>
-      </c>
-      <c r="M84" s="1" t="n">
-        <v>42.044</v>
-      </c>
-      <c r="N84" s="1"/>
-      <c r="O84" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P84" s="1" t="n">
-        <v>18.6</v>
-      </c>
-      <c r="Q84" s="1" t="n">
-        <v>19.592</v>
-      </c>
-      <c r="R84" s="1" t="n">
-        <v>0.991999999999999</v>
-      </c>
-      <c r="S84" s="1"/>
-      <c r="T84" s="1"/>
-      <c r="U84" s="1"/>
-      <c r="V84" s="1"/>
-      <c r="W84" s="1"/>
-      <c r="X84" s="1"/>
-      <c r="Y84" s="1"/>
-      <c r="Z84" s="1"/>
-      <c r="AA84" s="1"/>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
-      <c r="N85" s="1"/>
-      <c r="O85" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P85" s="1" t="n">
-        <v>11.16</v>
-      </c>
-      <c r="Q85" s="1" t="n">
-        <v>12.152</v>
-      </c>
-      <c r="R85" s="1" t="n">
-        <v>0.991999999999999</v>
-      </c>
-      <c r="S85" s="1"/>
-      <c r="T85" s="1"/>
-      <c r="U85" s="1"/>
-      <c r="V85" s="1"/>
-      <c r="W85" s="1"/>
-      <c r="X85" s="1"/>
-      <c r="Y85" s="1"/>
-      <c r="Z85" s="1"/>
-      <c r="AA85" s="1"/>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
-      <c r="N86" s="1"/>
-      <c r="O86" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="P86" s="1" t="n">
-        <v>3.72</v>
-      </c>
-      <c r="Q86" s="1" t="n">
-        <v>4.712</v>
-      </c>
-      <c r="R86" s="1" t="n">
-        <v>0.991999999999999</v>
-      </c>
-      <c r="S86" s="1"/>
-      <c r="T86" s="1"/>
-      <c r="U86" s="1"/>
-      <c r="V86" s="1"/>
-      <c r="W86" s="1"/>
-      <c r="X86" s="1"/>
-      <c r="Y86" s="1"/>
-      <c r="Z86" s="1"/>
-      <c r="AA86" s="1"/>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-      <c r="N87" s="1"/>
-      <c r="O87" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="P87" s="1" t="n">
-        <v>-3.72</v>
-      </c>
-      <c r="Q87" s="1" t="n">
-        <v>-4.718</v>
-      </c>
-      <c r="R87" s="1" t="n">
-        <v>-0.997999999999999</v>
-      </c>
-      <c r="S87" s="1"/>
-      <c r="T87" s="1"/>
-      <c r="U87" s="1"/>
-      <c r="V87" s="1"/>
-      <c r="W87" s="1"/>
-      <c r="X87" s="1"/>
-      <c r="Y87" s="1"/>
-      <c r="Z87" s="1"/>
-      <c r="AA87" s="1"/>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
-      <c r="M88" s="1"/>
-      <c r="N88" s="1"/>
-      <c r="O88" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="P88" s="1" t="n">
-        <v>-11.16</v>
-      </c>
-      <c r="Q88" s="1" t="n">
-        <v>-12.158</v>
-      </c>
-      <c r="R88" s="1" t="n">
-        <v>-0.997999999999999</v>
-      </c>
-      <c r="S88" s="1"/>
-      <c r="T88" s="1"/>
-      <c r="U88" s="1"/>
-      <c r="V88" s="1"/>
-      <c r="W88" s="1"/>
-      <c r="X88" s="1"/>
-      <c r="Y88" s="1"/>
-      <c r="Z88" s="1"/>
-      <c r="AA88" s="1"/>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
-      <c r="M89" s="1"/>
-      <c r="N89" s="1"/>
-      <c r="O89" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="P89" s="1" t="n">
-        <v>-18.6</v>
-      </c>
-      <c r="Q89" s="1" t="n">
-        <v>-19.598</v>
-      </c>
-      <c r="R89" s="1" t="n">
-        <v>-0.997999999999999</v>
-      </c>
-      <c r="S89" s="1"/>
-      <c r="T89" s="1"/>
-      <c r="U89" s="1"/>
-      <c r="V89" s="1"/>
-      <c r="W89" s="1"/>
-      <c r="X89" s="1"/>
-      <c r="Y89" s="1"/>
-      <c r="Z89" s="1"/>
-      <c r="AA89" s="1"/>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
-      <c r="M90" s="1"/>
-      <c r="N90" s="1"/>
-      <c r="O90" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="P90" s="1" t="n">
-        <v>-26.04</v>
-      </c>
-      <c r="Q90" s="1" t="n">
-        <v>-29.028</v>
-      </c>
-      <c r="R90" s="1" t="n">
-        <v>-2.988</v>
-      </c>
-      <c r="S90" s="1"/>
-      <c r="T90" s="1"/>
-      <c r="U90" s="1"/>
-      <c r="V90" s="1"/>
-      <c r="W90" s="1"/>
-      <c r="X90" s="1"/>
-      <c r="Y90" s="1"/>
-      <c r="Z90" s="1"/>
-      <c r="AA90" s="1"/>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
-      <c r="L91" s="1"/>
-      <c r="M91" s="1"/>
-      <c r="N91" s="1"/>
-      <c r="O91" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="P91" s="1" t="n">
-        <v>-33.48</v>
-      </c>
-      <c r="Q91" s="1" t="n">
-        <v>-36.468</v>
-      </c>
-      <c r="R91" s="1" t="n">
-        <v>-2.988</v>
-      </c>
-      <c r="S91" s="1"/>
-      <c r="T91" s="1"/>
-      <c r="U91" s="1"/>
-      <c r="V91" s="1"/>
-      <c r="W91" s="1"/>
-      <c r="X91" s="1"/>
-      <c r="Y91" s="1"/>
-      <c r="Z91" s="1"/>
-      <c r="AA91" s="1"/>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
-      <c r="O92" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="P92" s="1" t="n">
-        <v>-40.92</v>
-      </c>
-      <c r="Q92" s="1" t="n">
-        <v>-43.908</v>
-      </c>
-      <c r="R92" s="1" t="n">
-        <v>-2.988</v>
-      </c>
-      <c r="S92" s="1"/>
-      <c r="T92" s="1"/>
-      <c r="U92" s="1"/>
-      <c r="V92" s="1"/>
-      <c r="W92" s="1"/>
-      <c r="X92" s="1"/>
-      <c r="Y92" s="1"/>
-      <c r="Z92" s="1"/>
-      <c r="AA92" s="1"/>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
-      <c r="L93" s="1"/>
-      <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
-      <c r="O93" s="1"/>
-      <c r="P93" s="1"/>
-      <c r="Q93" s="1"/>
-      <c r="R93" s="1"/>
-      <c r="S93" s="1"/>
-      <c r="T93" s="1"/>
-      <c r="U93" s="1"/>
-      <c r="V93" s="1"/>
-      <c r="W93" s="1"/>
-      <c r="X93" s="1"/>
-      <c r="Y93" s="1"/>
-      <c r="Z93" s="1"/>
-      <c r="AA93" s="1"/>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
-      <c r="L94" s="1"/>
-      <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
-      <c r="O94" s="1"/>
-      <c r="P94" s="1"/>
-      <c r="Q94" s="1"/>
-      <c r="R94" s="1"/>
-      <c r="S94" s="1"/>
-      <c r="T94" s="1"/>
-      <c r="U94" s="1"/>
-      <c r="V94" s="1"/>
-      <c r="W94" s="1"/>
-      <c r="X94" s="1"/>
-      <c r="Y94" s="1"/>
-      <c r="Z94" s="1"/>
-      <c r="AA94" s="1"/>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C95" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D95" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E95" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F95" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G95" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H95" s="1" t="n">
-        <v>23.6</v>
-      </c>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K95" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L95" s="1" t="n">
-        <v>-29.557</v>
-      </c>
-      <c r="M95" s="1" t="n">
-        <v>-29.557</v>
-      </c>
-      <c r="N95" s="1"/>
-      <c r="O95" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P95" s="1" t="n">
-        <v>82.6</v>
-      </c>
-      <c r="Q95" s="1" t="n">
-        <v>48.265</v>
-      </c>
-      <c r="R95" s="1" t="n">
-        <v>-34.335</v>
-      </c>
-      <c r="S95" s="1"/>
-      <c r="T95" s="1"/>
-      <c r="U95" s="1"/>
-      <c r="V95" s="1"/>
-      <c r="W95" s="1"/>
-      <c r="X95" s="1"/>
-      <c r="Y95" s="1"/>
-      <c r="Z95" s="1"/>
-      <c r="AA95" s="1"/>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K96" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L96" s="1" t="n">
-        <v>-5.247</v>
-      </c>
-      <c r="M96" s="1" t="n">
-        <v>-5.247</v>
-      </c>
-      <c r="N96" s="1"/>
-      <c r="O96" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P96" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="Q96" s="1" t="n">
-        <v>24.665</v>
-      </c>
-      <c r="R96" s="1" t="n">
-        <v>-34.335</v>
-      </c>
-      <c r="S96" s="1"/>
-      <c r="T96" s="1"/>
-      <c r="U96" s="1"/>
-      <c r="V96" s="1"/>
-      <c r="W96" s="1"/>
-      <c r="X96" s="1"/>
-      <c r="Y96" s="1"/>
-      <c r="Z96" s="1"/>
-      <c r="AA96" s="1"/>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K97" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L97" s="1" t="n">
-        <v>19.063</v>
-      </c>
-      <c r="M97" s="1" t="n">
-        <v>19.063</v>
-      </c>
-      <c r="N97" s="1"/>
-      <c r="O97" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P97" s="1" t="n">
-        <v>35.4</v>
-      </c>
-      <c r="Q97" s="1" t="n">
-        <v>23.955</v>
-      </c>
-      <c r="R97" s="1" t="n">
-        <v>-11.445</v>
-      </c>
-      <c r="S97" s="1"/>
-      <c r="T97" s="1"/>
-      <c r="U97" s="1"/>
-      <c r="V97" s="1"/>
-      <c r="W97" s="1"/>
-      <c r="X97" s="1"/>
-      <c r="Y97" s="1"/>
-      <c r="Z97" s="1"/>
-      <c r="AA97" s="1"/>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K98" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L98" s="1" t="n">
-        <v>43.373</v>
-      </c>
-      <c r="M98" s="1" t="n">
-        <v>43.373</v>
-      </c>
-      <c r="N98" s="1"/>
-      <c r="O98" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P98" s="1" t="n">
-        <v>11.8</v>
-      </c>
-      <c r="Q98" s="1" t="n">
-        <v>0.354999999999999</v>
-      </c>
-      <c r="R98" s="1" t="n">
-        <v>-11.445</v>
-      </c>
-      <c r="S98" s="1"/>
-      <c r="T98" s="1"/>
-      <c r="U98" s="1"/>
-      <c r="V98" s="1"/>
-      <c r="W98" s="1"/>
-      <c r="X98" s="1"/>
-      <c r="Y98" s="1"/>
-      <c r="Z98" s="1"/>
-      <c r="AA98" s="1"/>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-      <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
-      <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
-      <c r="O99" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P99" s="1" t="n">
-        <v>-11.8</v>
-      </c>
-      <c r="Q99" s="1" t="n">
-        <v>-0.354999999999999</v>
-      </c>
-      <c r="R99" s="1" t="n">
-        <v>11.445</v>
-      </c>
-      <c r="S99" s="1"/>
-      <c r="T99" s="1"/>
-      <c r="U99" s="1"/>
-      <c r="V99" s="1"/>
-      <c r="W99" s="1"/>
-      <c r="X99" s="1"/>
-      <c r="Y99" s="1"/>
-      <c r="Z99" s="1"/>
-      <c r="AA99" s="1"/>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="P100" s="1" t="n">
-        <v>-35.4</v>
-      </c>
-      <c r="Q100" s="1" t="n">
-        <v>-23.955</v>
-      </c>
-      <c r="R100" s="1" t="n">
-        <v>11.445</v>
-      </c>
-      <c r="S100" s="1"/>
-      <c r="T100" s="1"/>
-      <c r="U100" s="1"/>
-      <c r="V100" s="1"/>
-      <c r="W100" s="1"/>
-      <c r="X100" s="1"/>
-      <c r="Y100" s="1"/>
-      <c r="Z100" s="1"/>
-      <c r="AA100" s="1"/>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="P101" s="1" t="n">
-        <v>-59</v>
-      </c>
-      <c r="Q101" s="1" t="n">
-        <v>-24.665</v>
-      </c>
-      <c r="R101" s="1" t="n">
-        <v>34.335</v>
-      </c>
-      <c r="S101" s="1"/>
-      <c r="T101" s="1"/>
-      <c r="U101" s="1"/>
-      <c r="V101" s="1"/>
-      <c r="W101" s="1"/>
-      <c r="X101" s="1"/>
-      <c r="Y101" s="1"/>
-      <c r="Z101" s="1"/>
-      <c r="AA101" s="1"/>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="P102" s="1" t="n">
-        <v>-82.6</v>
-      </c>
-      <c r="Q102" s="1" t="n">
-        <v>-48.265</v>
-      </c>
-      <c r="R102" s="1" t="n">
-        <v>34.335</v>
-      </c>
-      <c r="S102" s="1"/>
-      <c r="T102" s="1"/>
-      <c r="U102" s="1"/>
-      <c r="V102" s="1"/>
-      <c r="W102" s="1"/>
-      <c r="X102" s="1"/>
-      <c r="Y102" s="1"/>
-      <c r="Z102" s="1"/>
-      <c r="AA102" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>